<commit_message>
Verified binning and fixed bin bug
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tor.erik.larsen/Projects/afranalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504753D3-68EE-EF46-90C9-3159B7576E61}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC80569-669B-B549-B475-6349D6D50FA2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20860" yWindow="1760" windowWidth="32640" windowHeight="21740" xr2:uid="{D080EC81-5246-584F-868E-F782B5C598D6}"/>
+    <workbookView xWindow="16860" yWindow="1500" windowWidth="32640" windowHeight="21740" xr2:uid="{D080EC81-5246-584F-868E-F782B5C598D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -406,10 +406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84206DEA-568B-8148-8670-F978B04BDFAD}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>